<commit_message>
Fixed capitalization issue in lab template
</commit_message>
<xml_diff>
--- a/Load/ontology/script/lab_test_template_non-microbiology.xlsx
+++ b/Load/ontology/script/lab_test_template_non-microbiology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CA5256-4D72-4C40-8FE2-E43587F1AD8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D86D579-F640-C843-A5F2-05EEE5CE8ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -950,7 +950,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1036,7 @@
         <v>Ferritin (ng/ml), 2nd, at hospital</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f>TRIM(PROPER($B3)&amp;" test")</f>
+        <f t="shared" ref="I3:I5" si="0">TRIM(UPPER(LEFT(B3,1))&amp;RIGHT(B3,LEN(B3)-1)&amp;" test")</f>
         <v>Blood test</v>
       </c>
     </row>
@@ -1048,11 +1048,11 @@
         <v>15</v>
       </c>
       <c r="H4" s="2" t="str">
-        <f t="shared" ref="H4:H6" si="0">TRIM(UPPER(LEFT(C4,1))&amp;RIGHT(C4,LEN(C4)-1)&amp;IF(D4="",""," ("&amp;D4&amp;")")&amp;IF(E4="","",", "&amp;E4)&amp;IF(F4="","",", at "&amp;F4))</f>
+        <f t="shared" ref="H4:H6" si="1">TRIM(UPPER(LEFT(C4,1))&amp;RIGHT(C4,LEN(C4)-1)&amp;IF(D4="",""," ("&amp;D4&amp;")")&amp;IF(E4="","",", "&amp;E4)&amp;IF(F4="","",", at "&amp;F4))</f>
         <v>Leukopenia</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f t="shared" ref="I4:I6" si="1">TRIM(PROPER($B4)&amp;" test")</f>
+        <f t="shared" si="0"/>
         <v>Blood test</v>
       </c>
     </row>
@@ -1067,11 +1067,11 @@
         <v>17</v>
       </c>
       <c r="H5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Hematocrit (%)</v>
+      </c>
+      <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Hematocrit (%)</v>
-      </c>
-      <c r="I5" s="2" t="str">
-        <f t="shared" si="1"/>
         <v>Blood test</v>
       </c>
     </row>
@@ -1086,11 +1086,11 @@
         <v>22</v>
       </c>
       <c r="H6" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>TRIM(UPPER(LEFT(C6,1))&amp;RIGHT(C6,LEN(C6)-1)&amp;IF(D6="",""," ("&amp;D6&amp;")")&amp;IF(E6="","",", "&amp;E6)&amp;IF(F6="","",", at "&amp;F6))</f>
         <v>Adjusted mannitol (mmol/L)</v>
       </c>
       <c r="I6" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>TRIM(UPPER(LEFT(B6,1))&amp;RIGHT(B6,LEN(B6)-1)&amp;" test")</f>
         <v>Urine test</v>
       </c>
     </row>

</xml_diff>